<commit_message>
Added multiple loading functions and documented them.
</commit_message>
<xml_diff>
--- a/SAMPLES/zz_lista_volontera_23_24.xlsx
+++ b/SAMPLES/zz_lista_volontera_23_24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lobel\Documents\Lobel\Zlatni Zmaj\Evidencija\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lobel\Documents\Lobel\Zlatni Zmaj\Izvjesce\ZZ_Report_Analysis\SAMPLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C160CBA1-3C1F-4497-9F56-6BC36244F492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D9A292-0B8C-43DE-ADDD-3C18AB9FC9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{E4510751-5150-4AC6-8207-09F7448F3FDD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="252">
   <si>
     <t>svaki utorak i četvrtak 19:30 - 21:00</t>
   </si>
@@ -751,9 +751,6 @@
     <t>Veronika Grgić</t>
   </si>
   <si>
-    <t xml:space="preserve">PŠVPrelog </t>
-  </si>
-  <si>
     <t>Petar Celjak</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Sara Pobor</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1050,6 +1050,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,15 +1087,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1419,10 +1419,10 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="J8" s="4" t="s">
@@ -1487,11 +1487,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F55AA-7299-4F00-97AE-87619793A2A1}">
   <dimension ref="A1:BV139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="9" topLeftCell="G118" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="6" ySplit="9" topLeftCell="G115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,6 +1516,10 @@
       </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>COUNT(F:F)</f>
+        <v>91</v>
+      </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
@@ -1543,10 +1547,6 @@
       </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="F7">
-        <f>COUNTIF(G7:BB7,"&lt;&gt;")</f>
-        <v>48</v>
-      </c>
       <c r="G7" s="8" t="s">
         <v>17</v>
       </c>
@@ -2213,11 +2213,11 @@
         <f>SUM(F12:F65)</f>
         <v>311</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="12" spans="1:74" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -3641,11 +3641,11 @@
         <f>SUM(F70:F82)</f>
         <v>13</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
@@ -3803,11 +3803,11 @@
         <f>SUM(F87)</f>
         <v>4</v>
       </c>
-      <c r="C85" s="27" t="s">
+      <c r="C85" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
     </row>
     <row r="87" spans="1:64" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
@@ -3842,11 +3842,11 @@
         <f>SUM(F92:F115)</f>
         <v>37</v>
       </c>
-      <c r="C90" s="28" t="s">
+      <c r="C90" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
     </row>
     <row r="92" spans="1:64" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
@@ -4169,11 +4169,11 @@
         <f>SUM(F120)</f>
         <v>8</v>
       </c>
-      <c r="C118" s="29" t="s">
+      <c r="C118" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="D118" s="29"/>
-      <c r="E118" s="29"/>
+      <c r="D118" s="32"/>
+      <c r="E118" s="32"/>
     </row>
     <row r="120" spans="1:48" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
@@ -4219,11 +4219,11 @@
         <f>SUM(F125)</f>
         <v>0</v>
       </c>
-      <c r="C123" s="23" t="s">
+      <c r="C123" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D123" s="23"/>
-      <c r="E123" s="23"/>
+      <c r="D123" s="26"/>
+      <c r="E123" s="26"/>
     </row>
     <row r="125" spans="1:48" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
@@ -4246,13 +4246,16 @@
         <f>SUM(F130:F131)</f>
         <v>1</v>
       </c>
-      <c r="C128" s="24" t="s">
+      <c r="C128" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="D128" s="24"/>
-      <c r="E128" s="24"/>
+      <c r="D128" s="27"/>
+      <c r="E128" s="27"/>
     </row>
     <row r="130" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>251</v>
+      </c>
       <c r="E130" s="12" t="s">
         <v>186</v>
       </c>
@@ -4262,6 +4265,9 @@
       </c>
     </row>
     <row r="131" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>251</v>
+      </c>
       <c r="E131" t="s">
         <v>187</v>
       </c>
@@ -4282,11 +4288,11 @@
         <f>SUM(F136:F139)</f>
         <v>21</v>
       </c>
-      <c r="C134" s="22" t="s">
+      <c r="C134" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="D134" s="22"/>
-      <c r="E134" s="22"/>
+      <c r="D134" s="25"/>
+      <c r="E134" s="25"/>
     </row>
     <row r="136" spans="1:67" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
@@ -4403,13 +4409,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201BFF41-329F-4302-807C-28192EFA8C38}">
-  <dimension ref="A2:CK138"/>
+  <dimension ref="A1:CK138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="AK64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="BC108" sqref="BC108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4429,23 +4435,29 @@
     <col min="70" max="73" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <f>COUNT(E:E)</f>
+        <v>51</v>
+      </c>
+    </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>192</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>193</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <f>COUNTIF(E9:E92, "&gt;9")</f>
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <f>SUM(E9:E92)</f>
         <v>229</v>
       </c>
@@ -4458,13 +4470,9 @@
       <c r="Y3" t="s">
         <v>196</v>
       </c>
-      <c r="AC3" s="30" t="s">
+      <c r="AC3" t="s">
         <v>197</v>
       </c>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
     </row>
     <row r="4" spans="1:89" x14ac:dyDescent="0.25">
       <c r="F4" s="8">
@@ -4861,7 +4869,7 @@
         <v>198</v>
       </c>
       <c r="AV5" s="14">
-        <f t="shared" ref="AV5:CB5" si="3">COUNTIF(AV9:AV127,"da")</f>
+        <f t="shared" ref="AV5:BD5" si="3">COUNTIF(AV9:AV127,"da")</f>
         <v>3</v>
       </c>
       <c r="AW5" s="14">
@@ -4906,86 +4914,86 @@
         <v>198</v>
       </c>
       <c r="BH5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="BH5:BV5" si="4">COUNTIF(BH9:BH127,"da")</f>
         <v>5</v>
       </c>
       <c r="BI5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="BJ5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="BK5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="BL5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="BM5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="BN5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="BO5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BP5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="BQ5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BR5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="BS5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="BT5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="BU5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="BV5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="BW5" s="13" t="s">
         <v>198</v>
       </c>
       <c r="BX5" s="14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(BX9:BX127,"da")</f>
         <v>3</v>
       </c>
       <c r="BY5" s="14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(BY9:BY127,"da")</f>
         <v>2</v>
       </c>
       <c r="BZ5" s="14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(BZ9:BZ127,"da")</f>
         <v>5</v>
       </c>
       <c r="CA5" s="14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(CA9:CA127,"da")</f>
         <v>5</v>
       </c>
       <c r="CB5" s="14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF(CB9:CB127,"da")</f>
         <v>1</v>
       </c>
       <c r="CC5" s="13" t="s">
@@ -5230,11 +5238,11 @@
         <f>SUM(E9:E37)</f>
         <v>139</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -5598,7 +5606,7 @@
         <v>200</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" ref="E11:E18" si="4">COUNTIF(F11:ZZ11,"da")</f>
+        <f t="shared" ref="E11:E18" si="5">COUNTIF(F11:ZZ11,"da")</f>
         <v>15</v>
       </c>
       <c r="F11" s="14"/>
@@ -5723,7 +5731,7 @@
         <v>201</v>
       </c>
       <c r="E12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="F12" s="14"/>
@@ -5858,7 +5866,7 @@
         <v>202</v>
       </c>
       <c r="E13" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F13" s="14"/>
@@ -5953,7 +5961,7 @@
         <v>203</v>
       </c>
       <c r="E14" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F14" s="14"/>
@@ -6048,7 +6056,7 @@
         <v>204</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -6169,7 +6177,7 @@
         <v>205</v>
       </c>
       <c r="E16" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="F16" s="14" t="s">
@@ -6294,7 +6302,7 @@
         <v>108</v>
       </c>
       <c r="E17" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="F17" s="14"/>
@@ -6431,7 +6439,7 @@
         <v>206</v>
       </c>
       <c r="E18" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="F18" s="14" t="s">
@@ -6654,7 +6662,7 @@
         <v>207</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" ref="E20:E27" si="5">COUNTIF(F20:ZZ20,"da")</f>
+        <f t="shared" ref="E20:E27" si="6">COUNTIF(F20:ZZ20,"da")</f>
         <v>6</v>
       </c>
       <c r="F20" s="14"/>
@@ -6761,7 +6769,7 @@
         <v>208</v>
       </c>
       <c r="E21" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F21" s="14"/>
@@ -6856,7 +6864,7 @@
         <v>209</v>
       </c>
       <c r="E22" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="F22" s="14"/>
@@ -6959,7 +6967,7 @@
         <v>210</v>
       </c>
       <c r="E23" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F23" s="14"/>
@@ -7056,7 +7064,7 @@
         <v>211</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F24" s="14"/>
@@ -7151,7 +7159,7 @@
         <v>212</v>
       </c>
       <c r="E25" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="F25" s="14"/>
@@ -7250,7 +7258,7 @@
         <v>213</v>
       </c>
       <c r="E26" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F26" s="14"/>
@@ -7345,7 +7353,7 @@
         <v>214</v>
       </c>
       <c r="E27" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F27" s="14"/>
@@ -7532,7 +7540,7 @@
         <v>215</v>
       </c>
       <c r="E29" s="14">
-        <f t="shared" ref="E29:E37" si="6">COUNTIF(F29:ZZ29,"da")</f>
+        <f t="shared" ref="E29:E37" si="7">COUNTIF(F29:ZZ29,"da")</f>
         <v>6</v>
       </c>
       <c r="F29" s="14"/>
@@ -7639,7 +7647,7 @@
         <v>216</v>
       </c>
       <c r="E30" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F30" s="14"/>
@@ -7734,7 +7742,7 @@
         <v>217</v>
       </c>
       <c r="E31" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F31" s="14"/>
@@ -7837,7 +7845,7 @@
         <v>218</v>
       </c>
       <c r="E32" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="F32" s="14"/>
@@ -7942,7 +7950,7 @@
         <v>219</v>
       </c>
       <c r="E33" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="F33" s="14"/>
@@ -8047,7 +8055,7 @@
         <v>220</v>
       </c>
       <c r="E34" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F34" s="14"/>
@@ -8144,7 +8152,7 @@
         <v>221</v>
       </c>
       <c r="E35" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="F35" s="14"/>
@@ -8243,7 +8251,7 @@
         <v>222</v>
       </c>
       <c r="E36" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F36" s="14"/>
@@ -8338,7 +8346,7 @@
         <v>223</v>
       </c>
       <c r="E37" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F37" s="14"/>
@@ -8703,11 +8711,11 @@
         <f>SUM(E43)</f>
         <v>0</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -9256,11 +9264,11 @@
         <f>SUM(E49:E56)</f>
         <v>4</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
@@ -10473,11 +10481,11 @@
         <f>SUM(E62:E63)</f>
         <v>0</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
@@ -11121,11 +11129,11 @@
         <f>SUM(E69:E72)</f>
         <v>17</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="B67" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
@@ -11990,11 +11998,11 @@
         <f>SUM(E78:E92)</f>
         <v>69</v>
       </c>
-      <c r="B76" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="C76" s="31"/>
-      <c r="D76" s="31"/>
+      <c r="B76" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
       <c r="E76" s="14"/>
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
@@ -12177,10 +12185,10 @@
       </c>
       <c r="C78" s="17"/>
       <c r="D78" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E78" s="14">
-        <f t="shared" ref="E78:E84" si="7">COUNTIF(F78:ZZ78,"da")</f>
+        <f t="shared" ref="E78:E84" si="8">COUNTIF(F78:ZZ78,"da")</f>
         <v>0</v>
       </c>
       <c r="F78" s="14"/>
@@ -12272,10 +12280,10 @@
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E79" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="F79" s="14"/>
@@ -12437,10 +12445,10 @@
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E80" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F80" s="14"/>
@@ -12532,10 +12540,10 @@
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E81" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="F81" s="14"/>
@@ -12683,10 +12691,10 @@
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E82" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F82" s="14"/>
@@ -12778,10 +12786,10 @@
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
       <c r="D83" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E83" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F83" s="14"/>
@@ -12885,10 +12893,10 @@
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
       <c r="D84" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E84" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F84" s="14"/>
@@ -13072,10 +13080,10 @@
       </c>
       <c r="C86" s="17"/>
       <c r="D86" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E86" s="14">
-        <f t="shared" ref="E86:E92" si="8">COUNTIF(F86:ZZ86,"da")</f>
+        <f t="shared" ref="E86:E92" si="9">COUNTIF(F86:ZZ86,"da")</f>
         <v>0</v>
       </c>
       <c r="F86" s="14"/>
@@ -13167,10 +13175,10 @@
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
       <c r="D87" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E87" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F87" s="14"/>
@@ -13262,10 +13270,10 @@
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
       <c r="D88" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E88" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F88" s="14"/>
@@ -13357,10 +13365,10 @@
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
       <c r="D89" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E89" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F89" s="14"/>
@@ -13452,10 +13460,10 @@
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
       <c r="D90" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E90" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F90" s="14"/>
@@ -13547,10 +13555,10 @@
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
       <c r="D91" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E91" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F91" s="14"/>
@@ -13642,10 +13650,10 @@
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
       <c r="D92" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E92" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F92" s="14"/>
@@ -13734,86 +13742,6 @@
       <c r="CK92" s="15"/>
     </row>
     <row r="93" spans="2:89" x14ac:dyDescent="0.25">
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="14"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="14"/>
-      <c r="M93" s="14"/>
-      <c r="N93" s="14"/>
-      <c r="O93" s="14"/>
-      <c r="P93" s="14"/>
-      <c r="Q93" s="14"/>
-      <c r="R93" s="14"/>
-      <c r="S93" s="14"/>
-      <c r="T93" s="14"/>
-      <c r="U93" s="14"/>
-      <c r="V93" s="14"/>
-      <c r="W93" s="14"/>
-      <c r="X93" s="14"/>
-      <c r="Y93" s="14"/>
-      <c r="Z93" s="14"/>
-      <c r="AA93" s="14"/>
-      <c r="AB93" s="14"/>
-      <c r="AC93" s="14"/>
-      <c r="AD93" s="14"/>
-      <c r="AE93" s="14"/>
-      <c r="AF93" s="14"/>
-      <c r="AG93" s="14"/>
-      <c r="AH93" s="14"/>
-      <c r="AI93" s="14"/>
-      <c r="AJ93" s="14"/>
-      <c r="AK93" s="14"/>
-      <c r="AL93" s="14"/>
-      <c r="AM93" s="14"/>
-      <c r="AN93" s="14"/>
-      <c r="AO93" s="15"/>
-      <c r="AP93" s="14"/>
-      <c r="AQ93" s="14"/>
-      <c r="AR93" s="14"/>
-      <c r="AS93" s="14"/>
-      <c r="AT93" s="14"/>
-      <c r="AU93" s="14"/>
-      <c r="AV93" s="14"/>
-      <c r="AW93" s="14"/>
-      <c r="AX93" s="14"/>
-      <c r="AY93" s="14"/>
-      <c r="AZ93" s="14"/>
-      <c r="BA93" s="14"/>
-      <c r="BB93" s="14"/>
-      <c r="BC93" s="14"/>
-      <c r="BD93" s="14"/>
-      <c r="BE93" s="14"/>
-      <c r="BF93" s="14"/>
-      <c r="BG93" s="14"/>
-      <c r="BH93" s="14"/>
-      <c r="BI93" s="14"/>
-      <c r="BJ93" s="14"/>
-      <c r="BK93" s="14"/>
-      <c r="BL93" s="14"/>
-      <c r="BM93" s="14"/>
-      <c r="BN93" s="14"/>
-      <c r="BO93" s="14"/>
-      <c r="BP93" s="14"/>
-      <c r="BQ93" s="14"/>
-      <c r="BR93" s="15"/>
-      <c r="BS93" s="15"/>
-      <c r="BT93" s="15"/>
-      <c r="BU93" s="15"/>
-      <c r="BV93" s="15"/>
-      <c r="BW93" s="15"/>
-      <c r="BX93" s="15"/>
-      <c r="BY93" s="15"/>
-      <c r="BZ93" s="15"/>
-      <c r="CA93" s="15"/>
-      <c r="CB93" s="15"/>
-      <c r="CC93" s="15"/>
       <c r="CD93" s="15"/>
       <c r="CE93" s="15"/>
       <c r="CF93" s="15"/>
@@ -13824,86 +13752,6 @@
       <c r="CK93" s="15"/>
     </row>
     <row r="94" spans="2:89" x14ac:dyDescent="0.25">
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="14"/>
-      <c r="I94" s="14"/>
-      <c r="J94" s="14"/>
-      <c r="K94" s="14"/>
-      <c r="L94" s="14"/>
-      <c r="M94" s="14"/>
-      <c r="N94" s="14"/>
-      <c r="O94" s="14"/>
-      <c r="P94" s="14"/>
-      <c r="Q94" s="14"/>
-      <c r="R94" s="14"/>
-      <c r="S94" s="14"/>
-      <c r="T94" s="14"/>
-      <c r="U94" s="14"/>
-      <c r="V94" s="14"/>
-      <c r="W94" s="14"/>
-      <c r="X94" s="14"/>
-      <c r="Y94" s="14"/>
-      <c r="Z94" s="14"/>
-      <c r="AA94" s="14"/>
-      <c r="AB94" s="14"/>
-      <c r="AC94" s="14"/>
-      <c r="AD94" s="14"/>
-      <c r="AE94" s="14"/>
-      <c r="AF94" s="14"/>
-      <c r="AG94" s="14"/>
-      <c r="AH94" s="14"/>
-      <c r="AI94" s="14"/>
-      <c r="AJ94" s="14"/>
-      <c r="AK94" s="14"/>
-      <c r="AL94" s="14"/>
-      <c r="AM94" s="14"/>
-      <c r="AN94" s="14"/>
-      <c r="AO94" s="15"/>
-      <c r="AP94" s="14"/>
-      <c r="AQ94" s="14"/>
-      <c r="AR94" s="14"/>
-      <c r="AS94" s="14"/>
-      <c r="AT94" s="14"/>
-      <c r="AU94" s="14"/>
-      <c r="AV94" s="14"/>
-      <c r="AW94" s="14"/>
-      <c r="AX94" s="14"/>
-      <c r="AY94" s="14"/>
-      <c r="AZ94" s="14"/>
-      <c r="BA94" s="14"/>
-      <c r="BB94" s="14"/>
-      <c r="BC94" s="14"/>
-      <c r="BD94" s="14"/>
-      <c r="BE94" s="14"/>
-      <c r="BF94" s="14"/>
-      <c r="BG94" s="14"/>
-      <c r="BH94" s="14"/>
-      <c r="BI94" s="14"/>
-      <c r="BJ94" s="14"/>
-      <c r="BK94" s="14"/>
-      <c r="BL94" s="14"/>
-      <c r="BM94" s="14"/>
-      <c r="BN94" s="14"/>
-      <c r="BO94" s="14"/>
-      <c r="BP94" s="14"/>
-      <c r="BQ94" s="14"/>
-      <c r="BR94" s="15"/>
-      <c r="BS94" s="15"/>
-      <c r="BT94" s="15"/>
-      <c r="BU94" s="15"/>
-      <c r="BV94" s="15"/>
-      <c r="BW94" s="15"/>
-      <c r="BX94" s="15"/>
-      <c r="BY94" s="15"/>
-      <c r="BZ94" s="15"/>
-      <c r="CA94" s="15"/>
-      <c r="CB94" s="15"/>
-      <c r="CC94" s="15"/>
       <c r="CD94" s="15"/>
       <c r="CE94" s="15"/>
       <c r="CF94" s="15"/>
@@ -13914,86 +13762,6 @@
       <c r="CK94" s="15"/>
     </row>
     <row r="95" spans="2:89" x14ac:dyDescent="0.25">
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
-      <c r="J95" s="14"/>
-      <c r="K95" s="14"/>
-      <c r="L95" s="14"/>
-      <c r="M95" s="14"/>
-      <c r="N95" s="14"/>
-      <c r="O95" s="14"/>
-      <c r="P95" s="14"/>
-      <c r="Q95" s="14"/>
-      <c r="R95" s="14"/>
-      <c r="S95" s="14"/>
-      <c r="T95" s="14"/>
-      <c r="U95" s="14"/>
-      <c r="V95" s="14"/>
-      <c r="W95" s="14"/>
-      <c r="X95" s="14"/>
-      <c r="Y95" s="14"/>
-      <c r="Z95" s="14"/>
-      <c r="AA95" s="14"/>
-      <c r="AB95" s="14"/>
-      <c r="AC95" s="14"/>
-      <c r="AD95" s="14"/>
-      <c r="AE95" s="14"/>
-      <c r="AF95" s="14"/>
-      <c r="AG95" s="14"/>
-      <c r="AH95" s="14"/>
-      <c r="AI95" s="14"/>
-      <c r="AJ95" s="14"/>
-      <c r="AK95" s="14"/>
-      <c r="AL95" s="14"/>
-      <c r="AM95" s="14"/>
-      <c r="AN95" s="14"/>
-      <c r="AO95" s="15"/>
-      <c r="AP95" s="14"/>
-      <c r="AQ95" s="14"/>
-      <c r="AR95" s="14"/>
-      <c r="AS95" s="14"/>
-      <c r="AT95" s="14"/>
-      <c r="AU95" s="14"/>
-      <c r="AV95" s="14"/>
-      <c r="AW95" s="14"/>
-      <c r="AX95" s="14"/>
-      <c r="AY95" s="14"/>
-      <c r="AZ95" s="14"/>
-      <c r="BA95" s="14"/>
-      <c r="BB95" s="14"/>
-      <c r="BC95" s="14"/>
-      <c r="BD95" s="14"/>
-      <c r="BE95" s="14"/>
-      <c r="BF95" s="14"/>
-      <c r="BG95" s="14"/>
-      <c r="BH95" s="14"/>
-      <c r="BI95" s="14"/>
-      <c r="BJ95" s="14"/>
-      <c r="BK95" s="14"/>
-      <c r="BL95" s="14"/>
-      <c r="BM95" s="14"/>
-      <c r="BN95" s="14"/>
-      <c r="BO95" s="14"/>
-      <c r="BP95" s="14"/>
-      <c r="BQ95" s="14"/>
-      <c r="BR95" s="15"/>
-      <c r="BS95" s="15"/>
-      <c r="BT95" s="15"/>
-      <c r="BU95" s="15"/>
-      <c r="BV95" s="15"/>
-      <c r="BW95" s="15"/>
-      <c r="BX95" s="15"/>
-      <c r="BY95" s="15"/>
-      <c r="BZ95" s="15"/>
-      <c r="CA95" s="15"/>
-      <c r="CB95" s="15"/>
-      <c r="CC95" s="15"/>
       <c r="CD95" s="15"/>
       <c r="CE95" s="15"/>
       <c r="CF95" s="15"/>
@@ -17480,15 +17248,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D11:V18">
     <sortCondition ref="D11:D18"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B67:D67"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>